<commit_message>
updated files datasheet and app java files
</commit_message>
<xml_diff>
--- a/sample/src/main/resources/Datasheet.xlsx
+++ b/sample/src/main/resources/Datasheet.xlsx
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>https://www.softwaretestingmaterial.com/</t>
-  </si>
-  <si>
-    <t>urls</t>
   </si>
   <si>
     <t>https://www.google.com/</t>
@@ -372,9 +369,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -382,13 +381,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -396,16 +395,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>